<commit_message>
104245 - wip, added unit tests
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.Operations.Reports.Reports/Templates/FundingClaimsProviderSubmissionsReport1920Template.xlsx
+++ b/src/ESFA.DC.Operations.Reports.Reports/Templates/FundingClaimsProviderSubmissionsReport1920Template.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VSTS\DCT\DC-Operations-Reports\src\ESFA.DC.Operations.Reports.Reports\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D91B80-F9B3-4136-93D2-B5077AF13BD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D977D84-FF46-4201-9DA9-06B4F492A5E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="1819 FC Provider Submissions " sheetId="1" r:id="rId1"/>
+    <sheet name="1920 FC Provider Submissions " sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
   <si>
     <t>UKPRN</t>
   </si>
@@ -34,21 +34,6 @@
     <t>Returned In Current Period</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">No of Returning Unexpected Providers: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>6</t>
-    </r>
-  </si>
-  <si>
     <t>Date Latest Claim Submitted</t>
   </si>
   <si>
@@ -106,68 +91,86 @@
     <t>&amp;=FundingClaimsInfo.NoOfExpectedProvidersNotReturning</t>
   </si>
   <si>
-    <t>&amp;=FundingClaimsInfo.NoOfReturningUnexpectedProviders</t>
+    <t>&amp;=FundingClaimsInfo.FundingClaimsSubmissionsDetails.UkPrn</t>
+  </si>
+  <si>
+    <t>&amp;=FundingClaimsInfo.FundingClaimsSubmissionsDetails.ProviderName</t>
+  </si>
+  <si>
+    <t>&amp;=FundingClaimsInfo.FundingClaimsSubmissionsDetails.ExpectedToReturnInCurrentPeriod</t>
+  </si>
+  <si>
+    <t>&amp;=FundingClaimsInfo.FundingClaimsSubmissionsDetails.ReturnedInCurrentPeriod</t>
+  </si>
+  <si>
+    <t>&amp;=FundingClaimsInfo.FundingClaimsSubmissionsDetails.DateLatestClaimSubmitted</t>
+  </si>
+  <si>
+    <t>&amp;=FundingClaimsInfo.FundingClaimsSubmissionsDetails.ALLBC1920ContractValue</t>
+  </si>
+  <si>
+    <t>&amp;=FundingClaimsInfo.FundingClaimsSubmissionsDetails.ALLBC1920Claimed</t>
+  </si>
+  <si>
+    <t>&amp;=FundingClaimsInfo.FundingClaimsSubmissionsDetails.AEBCASCL1920ContractValue</t>
+  </si>
+  <si>
+    <t>&amp;=FundingClaimsInfo.FundingClaimsSubmissionsDetails.AEBCASCL1920Claimed</t>
+  </si>
+  <si>
+    <t>&amp;=FundingClaimsInfo.FundingClaimsSubmissionsDetails.AEBC19TRN1920ContractValue</t>
+  </si>
+  <si>
+    <t>&amp;=FundingClaimsInfo.FundingClaimsSubmissionsDetails.AEBC19TRN1920Claimed</t>
+  </si>
+  <si>
+    <t>&amp;=FundingClaimsInfo.FundingClaimsSubmissionsDetails.AEBASLS1920ProcuredContractValue</t>
+  </si>
+  <si>
+    <t>&amp;=FundingClaimsInfo.FundingClaimsSubmissionsDetails.AEBASLS1920ProcuredClaimed</t>
+  </si>
+  <si>
+    <t>&amp;=FundingClaimsInfo.FundingClaimsSubmissionsDetails.AEB19TRLS1920ProcuredContractValue</t>
+  </si>
+  <si>
+    <t>&amp;=FundingClaimsInfo.FundingClaimsSubmissionsDetails.AEB19TRLS1920ProcuredClaimed</t>
+  </si>
+  <si>
+    <t>&amp;=FundingClaimsInfo.FundingClaimsSubmissionsDetails.ED1920ContractValue1619</t>
+  </si>
+  <si>
+    <t>&amp;=FundingClaimsInfo.FundingClaimsSubmissionsDetails.ED1920Claimed1619</t>
+  </si>
+  <si>
+    <t>Total No of Returning Providers:</t>
+  </si>
+  <si>
+    <t>No of Providers Expected to Return:</t>
+  </si>
+  <si>
+    <t>No of Expected Providers Not Returning:</t>
+  </si>
+  <si>
+    <t>No of Returning Expected Providers:</t>
+  </si>
+  <si>
+    <t>No of Returning Unexpected Providers:</t>
+  </si>
+  <si>
+    <t>Report Run:</t>
+  </si>
+  <si>
+    <t>Funding Claim:</t>
   </si>
   <si>
     <t>&amp;=FundingClaimsInfo.FundingClaim</t>
-  </si>
-  <si>
-    <t>&amp;=FundingClaimsInfo.FundingClaimsSubmissionsDetails.UkPrn</t>
-  </si>
-  <si>
-    <t>&amp;=FundingClaimsInfo.FundingClaimsSubmissionsDetails.ProviderName</t>
-  </si>
-  <si>
-    <t>&amp;=FundingClaimsInfo.FundingClaimsSubmissionsDetails.ExpectedToReturnInCurrentPeriod</t>
-  </si>
-  <si>
-    <t>&amp;=FundingClaimsInfo.FundingClaimsSubmissionsDetails.ReturnedInCurrentPeriod</t>
-  </si>
-  <si>
-    <t>&amp;=FundingClaimsInfo.FundingClaimsSubmissionsDetails.DateLatestClaimSubmitted</t>
-  </si>
-  <si>
-    <t>&amp;=FundingClaimsInfo.FundingClaimsSubmissionsDetails.ALLBC1920ContractValue</t>
-  </si>
-  <si>
-    <t>&amp;=FundingClaimsInfo.FundingClaimsSubmissionsDetails.ALLBC1920Claimed</t>
-  </si>
-  <si>
-    <t>&amp;=FundingClaimsInfo.FundingClaimsSubmissionsDetails.AEBCASCL1920ContractValue</t>
-  </si>
-  <si>
-    <t>&amp;=FundingClaimsInfo.FundingClaimsSubmissionsDetails.AEBCASCL1920Claimed</t>
-  </si>
-  <si>
-    <t>&amp;=FundingClaimsInfo.FundingClaimsSubmissionsDetails.AEBC19TRN1920ContractValue</t>
-  </si>
-  <si>
-    <t>&amp;=FundingClaimsInfo.FundingClaimsSubmissionsDetails.AEBC19TRN1920Claimed</t>
-  </si>
-  <si>
-    <t>&amp;=FundingClaimsInfo.FundingClaimsSubmissionsDetails.AEBASLS1920ProcuredContractValue</t>
-  </si>
-  <si>
-    <t>&amp;=FundingClaimsInfo.FundingClaimsSubmissionsDetails.AEBASLS1920ProcuredClaimed</t>
-  </si>
-  <si>
-    <t>&amp;=FundingClaimsInfo.FundingClaimsSubmissionsDetails.AEB19TRLS1920ProcuredContractValue</t>
-  </si>
-  <si>
-    <t>&amp;=FundingClaimsInfo.FundingClaimsSubmissionsDetails.AEB19TRLS1920ProcuredClaimed</t>
-  </si>
-  <si>
-    <t>&amp;=FundingClaimsInfo.FundingClaimsSubmissionsDetails.ED1920ContractValue1619</t>
-  </si>
-  <si>
-    <t>&amp;=FundingClaimsInfo.FundingClaimsSubmissionsDetails.ED1920Claimed1619</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -188,19 +191,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color theme="0"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -209,6 +199,23 @@
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -232,7 +239,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -256,6 +263,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="thin">
         <color rgb="FFD3D3D3"/>
@@ -263,9 +285,20 @@
       <top style="thin">
         <color rgb="FFD3D3D3"/>
       </top>
-      <bottom style="thin">
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFD3D3D3"/>
-      </bottom>
+      </left>
+      <right style="thin">
+        <color rgb="FFD3D3D3"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFD3D3D3"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -274,8 +307,43 @@
       <top style="thin">
         <color rgb="FFD3D3D3"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
-        <color rgb="FFD3D3D3"/>
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -283,58 +351,62 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="22" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="14">
     <dxf>
       <fill>
         <patternFill>
@@ -345,6 +417,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF6699"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
@@ -423,111 +502,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6699"/>
         </patternFill>
       </fill>
     </dxf>
@@ -945,10 +919,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:Y11"/>
+  <dimension ref="B1:Y9"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11:O11"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -956,305 +930,306 @@
     <col min="1" max="1" width="3.42578125" customWidth="1"/>
     <col min="2" max="2" width="0.42578125" customWidth="1"/>
     <col min="3" max="3" width="13.28515625" customWidth="1"/>
-    <col min="4" max="4" width="29.5703125" customWidth="1"/>
-    <col min="5" max="5" width="2.28515625" customWidth="1"/>
-    <col min="6" max="6" width="22" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="6" max="6" width="36.5703125" customWidth="1"/>
     <col min="7" max="7" width="13.7109375" customWidth="1"/>
     <col min="8" max="8" width="1.42578125" customWidth="1"/>
     <col min="9" max="9" width="0" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="12.140625" customWidth="1"/>
     <col min="11" max="11" width="9.85546875" customWidth="1"/>
     <col min="12" max="12" width="0" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="9.42578125" customWidth="1"/>
-    <col min="14" max="14" width="18.42578125" style="4" customWidth="1"/>
+    <col min="13" max="13" width="13.140625" customWidth="1"/>
+    <col min="14" max="14" width="18.42578125" style="2" customWidth="1"/>
     <col min="15" max="15" width="18" customWidth="1"/>
-    <col min="16" max="17" width="18" style="5" customWidth="1"/>
-    <col min="18" max="19" width="18" style="9" customWidth="1"/>
-    <col min="20" max="20" width="15.28515625" style="4" customWidth="1"/>
+    <col min="16" max="17" width="18" style="3" customWidth="1"/>
+    <col min="18" max="19" width="18" style="5" customWidth="1"/>
+    <col min="20" max="20" width="15.28515625" style="2" customWidth="1"/>
     <col min="21" max="21" width="14.28515625" style="1" customWidth="1"/>
-    <col min="22" max="22" width="15.28515625" style="9" customWidth="1"/>
-    <col min="23" max="23" width="14.28515625" style="9" customWidth="1"/>
-    <col min="24" max="24" width="17.42578125" style="7" customWidth="1"/>
-    <col min="25" max="25" width="18" style="7" customWidth="1"/>
+    <col min="22" max="22" width="15.28515625" style="5" customWidth="1"/>
+    <col min="23" max="23" width="14.28515625" style="5" customWidth="1"/>
+    <col min="24" max="24" width="17.42578125" style="4" customWidth="1"/>
+    <col min="25" max="25" width="18" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:25" ht="11.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:25" ht="23.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="15"/>
-      <c r="P2" s="15"/>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="15"/>
-      <c r="S2" s="15"/>
-      <c r="T2" s="15"/>
-      <c r="U2" s="15"/>
-      <c r="V2" s="15"/>
-      <c r="W2" s="15"/>
+      <c r="C2" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="19"/>
+      <c r="S2" s="19"/>
+      <c r="T2" s="19"/>
+      <c r="U2" s="19"/>
+      <c r="V2" s="19"/>
+      <c r="W2" s="19"/>
       <c r="X2"/>
       <c r="Y2"/>
     </row>
-    <row r="3" spans="2:25" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="2:25" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="16" t="s">
+    <row r="3" spans="2:25" s="6" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
+    </row>
+    <row r="4" spans="2:25" s="6" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="20"/>
+      <c r="E4" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="17" t="s">
+      <c r="F4" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="2:25" s="6" customFormat="1" ht="23.85" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="20"/>
+      <c r="E5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="K5" s="21"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="21"/>
+      <c r="N5" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="2:25" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="2:25" ht="22.35" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="2:25" ht="51" x14ac:dyDescent="0.25">
+      <c r="B8" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="15"/>
+      <c r="D8" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="17"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="I8" s="17"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="L8" s="17"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="O8" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="P8" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q8" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="R8" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="S8" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="T8" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="U8" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="V8" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="W8" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="X8" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y8" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="C9" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13"/>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="13"/>
-      <c r="R4" s="13"/>
-    </row>
-    <row r="5" spans="2:25" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="2:25" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="16"/>
-      <c r="F6" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="17"/>
-    </row>
-    <row r="7" spans="2:25" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="2:25" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="15"/>
-      <c r="F8" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" s="15"/>
-      <c r="I8" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="J8" s="12"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
-      <c r="M8" s="11"/>
-    </row>
-    <row r="9" spans="2:25" ht="22.35" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="2:25" ht="51" x14ac:dyDescent="0.25">
-      <c r="B10" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="E10" s="20"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="H10" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="I10" s="20"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="L10" s="20"/>
-      <c r="M10" s="19"/>
-      <c r="N10" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="O10" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="P10" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q10" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="R10" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="S10" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="T10" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="U10" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="V10" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="W10" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="X10" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="Y10" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="C11" s="13" t="s">
+      <c r="H9" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="D11" t="s">
+      <c r="I9" s="24"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="G11" t="s">
+      <c r="L9" s="24"/>
+      <c r="M9" s="25"/>
+      <c r="N9" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="J11" t="s">
+      <c r="O9" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="K11" t="s">
+      <c r="P9" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="N11" s="4" t="s">
+      <c r="Q9" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="O11" t="s">
+      <c r="R9" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="P11" s="5" t="s">
+      <c r="S9" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="Q11" s="5" t="s">
+      <c r="T9" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="R11" s="9" t="s">
+      <c r="U9" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="S11" s="9" t="s">
+      <c r="V9" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="T11" s="4" t="s">
+      <c r="W9" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="U11" s="1" t="s">
+      <c r="X9" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="V11" s="9" t="s">
+      <c r="Y9" s="13" t="s">
         <v>39</v>
-      </c>
-      <c r="W11" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="X11" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y11" s="7" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="11">
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="K8:M8"/>
     <mergeCell ref="C2:W2"/>
     <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="F4:J4"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="K10:M10"/>
-    <mergeCell ref="F6:J6"/>
-    <mergeCell ref="K6:O6"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="J5:M5"/>
+    <mergeCell ref="G3:M3"/>
   </mergeCells>
-  <conditionalFormatting sqref="J11">
-    <cfRule type="expression" dxfId="27" priority="15">
-      <formula>AND($G11="YES", $J11="No")</formula>
+  <conditionalFormatting sqref="N9:O9">
+    <cfRule type="expression" dxfId="13" priority="11">
+      <formula>AND($N9=0, $O9&lt;&gt;0)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="12">
+      <formula>AND($N9&lt;&gt;0, $O9=0)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G11:J11">
-    <cfRule type="expression" dxfId="26" priority="14">
-      <formula>AND($G11="No", $J11="No")</formula>
+  <conditionalFormatting sqref="P9:Q9">
+    <cfRule type="expression" dxfId="11" priority="9">
+      <formula>AND($P9=0, $Q9&lt;&gt;0)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="10">
+      <formula>AND($P9&lt;&gt;0, $Q9=0)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N11:O11">
-    <cfRule type="expression" dxfId="25" priority="12">
-      <formula>AND($N11&lt;&gt;0, $O11=0)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="14" priority="11">
-      <formula>AND($N11=0, $O11&lt;&gt;0)</formula>
+  <conditionalFormatting sqref="R9:S9">
+    <cfRule type="expression" dxfId="9" priority="7">
+      <formula>AND($R9=0, $S9&lt;&gt;0)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="8">
+      <formula>AND($R9&lt;&gt;0, $S9=0)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P11:Q11">
-    <cfRule type="expression" dxfId="24" priority="10">
-      <formula>AND($P11&lt;&gt;0, $Q11=0)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="23" priority="9">
-      <formula>AND($P11=0, $Q11&lt;&gt;0)</formula>
+  <conditionalFormatting sqref="T9:U9">
+    <cfRule type="expression" dxfId="7" priority="5">
+      <formula>AND($T9=0, $U9&lt;&gt;0)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="6">
+      <formula>AND($T9&lt;&gt;0, $U9=0)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R11:S11">
-    <cfRule type="expression" dxfId="22" priority="8">
-      <formula>AND($R11&lt;&gt;0, $S11=0)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="21" priority="7">
-      <formula>AND($R11=0, $S11&lt;&gt;0)</formula>
+  <conditionalFormatting sqref="V9:W9">
+    <cfRule type="expression" dxfId="5" priority="3">
+      <formula>AND($V9=0, $W9&lt;&gt;0)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="4">
+      <formula>AND($V9&lt;&gt;0, $W9=0)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T11:U11">
-    <cfRule type="expression" dxfId="20" priority="6">
-      <formula>AND($T11&lt;&gt;0, $U11=0)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="19" priority="5">
-      <formula>AND($T11=0, $U11&lt;&gt;0)</formula>
+  <conditionalFormatting sqref="X9:Y9">
+    <cfRule type="expression" dxfId="3" priority="1">
+      <formula>AND($X9=0, $Y9&lt;&gt;0)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>AND($X9&lt;&gt;0, $Y9=0)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V11:W11">
-    <cfRule type="expression" dxfId="18" priority="4">
-      <formula>AND($V11&lt;&gt;0, $W11=0)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="17" priority="3">
-      <formula>AND($V11=0, $W11&lt;&gt;0)</formula>
+  <conditionalFormatting sqref="H9">
+    <cfRule type="expression" dxfId="1" priority="16">
+      <formula>AND($G9="YES", $H9="No")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X11:Y11">
-    <cfRule type="expression" dxfId="16" priority="2">
-      <formula>AND($X11&lt;&gt;0, $Y11=0)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="15" priority="1">
-      <formula>AND($X11=0, $Y11&lt;&gt;0)</formula>
+  <conditionalFormatting sqref="G9:H9">
+    <cfRule type="expression" dxfId="0" priority="17">
+      <formula>AND($G9="No", $H9="No")</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="1" right="1" top="1" bottom="1" header="1" footer="1"/>

</xml_diff>

<commit_message>
104245 - 1920 FundingClaimsProviderSubmissionsReport
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.Operations.Reports.Reports/Templates/FundingClaimsProviderSubmissionsReport1920Template.xlsx
+++ b/src/ESFA.DC.Operations.Reports.Reports/Templates/FundingClaimsProviderSubmissionsReport1920Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VSTS\DCT\DC-Operations-Reports\src\ESFA.DC.Operations.Reports.Reports\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D977D84-FF46-4201-9DA9-06B4F492A5E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76902557-6B85-4404-B434-7B70387444EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>UKPRN</t>
   </si>
@@ -160,10 +160,19 @@
     <t>Report Run:</t>
   </si>
   <si>
-    <t>Funding Claim:</t>
-  </si>
-  <si>
     <t>&amp;=FundingClaimsInfo.FundingClaim</t>
+  </si>
+  <si>
+    <t>COVID-19 Declaration Response</t>
+  </si>
+  <si>
+    <t>&amp;=FundingClaimsInfo.FundingClaimsSubmissionsDetails.CovidResponse</t>
+  </si>
+  <si>
+    <t>Claim Period:</t>
+  </si>
+  <si>
+    <t>&amp;=FundingClaimsInfo.NoOfReturningUnexpectedProviders</t>
   </si>
 </sst>
 </file>
@@ -351,7 +360,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -362,20 +371,25 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="22" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
@@ -396,17 +410,22 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="22" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="15">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -919,10 +938,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:Y9"/>
+  <dimension ref="B1:Z9"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -931,7 +950,7 @@
     <col min="2" max="2" width="0.42578125" customWidth="1"/>
     <col min="3" max="3" width="13.28515625" customWidth="1"/>
     <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" customWidth="1"/>
     <col min="6" max="6" width="36.5703125" customWidth="1"/>
     <col min="7" max="7" width="13.7109375" customWidth="1"/>
     <col min="8" max="8" width="1.42578125" customWidth="1"/>
@@ -940,296 +959,316 @@
     <col min="11" max="11" width="9.85546875" customWidth="1"/>
     <col min="12" max="12" width="0" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="13.140625" customWidth="1"/>
-    <col min="14" max="14" width="18.42578125" style="2" customWidth="1"/>
-    <col min="15" max="15" width="18" customWidth="1"/>
-    <col min="16" max="17" width="18" style="3" customWidth="1"/>
-    <col min="18" max="19" width="18" style="5" customWidth="1"/>
-    <col min="20" max="20" width="15.28515625" style="2" customWidth="1"/>
-    <col min="21" max="21" width="14.28515625" style="1" customWidth="1"/>
-    <col min="22" max="22" width="15.28515625" style="5" customWidth="1"/>
-    <col min="23" max="23" width="14.28515625" style="5" customWidth="1"/>
-    <col min="24" max="24" width="17.42578125" style="4" customWidth="1"/>
-    <col min="25" max="25" width="18" style="4" customWidth="1"/>
+    <col min="14" max="14" width="21.28515625" style="13" customWidth="1"/>
+    <col min="15" max="15" width="18.42578125" style="2" customWidth="1"/>
+    <col min="16" max="16" width="18" customWidth="1"/>
+    <col min="17" max="18" width="18" style="3" customWidth="1"/>
+    <col min="19" max="20" width="18" style="5" customWidth="1"/>
+    <col min="21" max="21" width="15.28515625" style="2" customWidth="1"/>
+    <col min="22" max="22" width="14.28515625" style="1" customWidth="1"/>
+    <col min="23" max="23" width="15.28515625" style="5" customWidth="1"/>
+    <col min="24" max="24" width="14.28515625" style="5" customWidth="1"/>
+    <col min="25" max="25" width="17.42578125" style="4" customWidth="1"/>
+    <col min="26" max="26" width="18" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:25" ht="11.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:25" ht="23.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="18" t="s">
+    <row r="1" spans="2:26" ht="11.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:26" ht="23.85" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="19"/>
-      <c r="S2" s="19"/>
-      <c r="T2" s="19"/>
-      <c r="U2" s="19"/>
-      <c r="V2" s="19"/>
-      <c r="W2" s="19"/>
-      <c r="X2"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
+      <c r="P2" s="24"/>
+      <c r="Q2" s="24"/>
+      <c r="R2" s="24"/>
+      <c r="S2" s="24"/>
+      <c r="T2" s="24"/>
+      <c r="U2" s="24"/>
+      <c r="V2" s="24"/>
+      <c r="W2" s="24"/>
+      <c r="X2" s="24"/>
       <c r="Y2"/>
+      <c r="Z2"/>
     </row>
-    <row r="3" spans="2:25" s="6" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="9" t="s">
+    <row r="3" spans="2:26" s="6" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="H3" s="25"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="G3" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="22"/>
-      <c r="K3" s="22"/>
-      <c r="L3" s="22"/>
-      <c r="M3" s="22"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="27"/>
+      <c r="M3" s="27"/>
+      <c r="N3" s="14"/>
+      <c r="Q3" s="13"/>
     </row>
-    <row r="4" spans="2:25" s="6" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="20" t="s">
+    <row r="4" spans="2:26" s="6" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="D4" s="20"/>
+      <c r="D4" s="25"/>
       <c r="E4" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="8" t="s">
         <v>42</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>22</v>
       </c>
+      <c r="N4" s="13"/>
     </row>
-    <row r="5" spans="2:25" s="6" customFormat="1" ht="23.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="20" t="s">
+    <row r="5" spans="2:26" s="6" customFormat="1" ht="23.85" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="D5" s="20"/>
+      <c r="D5" s="25"/>
       <c r="E5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="8" t="s">
         <v>43</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="J5" s="21" t="s">
+      <c r="J5" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="K5" s="21"/>
-      <c r="L5" s="21"/>
-      <c r="M5" s="21"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
       <c r="N5" s="7" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
     </row>
-    <row r="6" spans="2:25" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="2:25" ht="22.35" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="2:25" ht="51" x14ac:dyDescent="0.25">
-      <c r="B8" s="14" t="s">
+    <row r="6" spans="2:26" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="2:26" ht="22.35" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="2:26" ht="51" x14ac:dyDescent="0.25">
+      <c r="B8" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="15"/>
-      <c r="D8" s="16" t="s">
+      <c r="C8" s="20"/>
+      <c r="D8" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="E8" s="17"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="12" t="s">
+      <c r="E8" s="22"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="H8" s="16" t="s">
+      <c r="H8" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="I8" s="17"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="16" t="s">
+      <c r="I8" s="22"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="L8" s="17"/>
-      <c r="M8" s="15"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="20"/>
       <c r="N8" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="O8" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="O8" s="12" t="s">
+      <c r="P8" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="P8" s="12" t="s">
+      <c r="Q8" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="Q8" s="12" t="s">
+      <c r="R8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="R8" s="12" t="s">
+      <c r="S8" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="S8" s="12" t="s">
+      <c r="T8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="T8" s="12" t="s">
+      <c r="U8" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="U8" s="12" t="s">
+      <c r="V8" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="V8" s="12" t="s">
+      <c r="W8" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="W8" s="12" t="s">
+      <c r="X8" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="X8" s="12" t="s">
+      <c r="Y8" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="Y8" s="12" t="s">
+      <c r="Z8" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="C9" s="13" t="s">
+    <row r="9" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="C9" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13" t="s">
+      <c r="E9" s="17"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="H9" s="23" t="s">
+      <c r="H9" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="I9" s="24"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="23" t="s">
+      <c r="I9" s="17"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="L9" s="24"/>
-      <c r="M9" s="25"/>
-      <c r="N9" s="13" t="s">
+      <c r="L9" s="17"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="O9" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="O9" s="13" t="s">
+      <c r="P9" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="P9" s="13" t="s">
+      <c r="Q9" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="Q9" s="13" t="s">
+      <c r="R9" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="R9" s="13" t="s">
+      <c r="S9" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="S9" s="13" t="s">
+      <c r="T9" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="T9" s="13" t="s">
+      <c r="U9" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="U9" s="13" t="s">
+      <c r="V9" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="V9" s="13" t="s">
+      <c r="W9" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="W9" s="13" t="s">
+      <c r="X9" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="X9" s="13" t="s">
+      <c r="Y9" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="Y9" s="13" t="s">
+      <c r="Z9" s="10" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="14">
+    <mergeCell ref="C2:X2"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="J5:M5"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="J3:M3"/>
+    <mergeCell ref="D3:F3"/>
     <mergeCell ref="H9:J9"/>
     <mergeCell ref="K9:M9"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="D8:F8"/>
     <mergeCell ref="H8:J8"/>
     <mergeCell ref="K8:M8"/>
-    <mergeCell ref="C2:W2"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="J5:M5"/>
-    <mergeCell ref="G3:M3"/>
+    <mergeCell ref="D9:F9"/>
   </mergeCells>
-  <conditionalFormatting sqref="N9:O9">
-    <cfRule type="expression" dxfId="13" priority="11">
-      <formula>AND($N9=0, $O9&lt;&gt;0)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="12" priority="12">
-      <formula>AND($N9&lt;&gt;0, $O9=0)</formula>
+  <conditionalFormatting sqref="O9:P9">
+    <cfRule type="expression" dxfId="14" priority="12">
+      <formula>AND($O9=0, $P9&lt;&gt;0)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="13">
+      <formula>AND($O9&lt;&gt;0, $P9=0)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P9:Q9">
-    <cfRule type="expression" dxfId="11" priority="9">
-      <formula>AND($P9=0, $Q9&lt;&gt;0)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="10">
-      <formula>AND($P9&lt;&gt;0, $Q9=0)</formula>
+  <conditionalFormatting sqref="Q9:R9">
+    <cfRule type="expression" dxfId="12" priority="10">
+      <formula>AND($Q9=0, $R9&lt;&gt;0)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="11" priority="11">
+      <formula>AND($Q9&lt;&gt;0, $R9=0)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R9:S9">
-    <cfRule type="expression" dxfId="9" priority="7">
-      <formula>AND($R9=0, $S9&lt;&gt;0)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="8" priority="8">
-      <formula>AND($R9&lt;&gt;0, $S9=0)</formula>
+  <conditionalFormatting sqref="S9:T9">
+    <cfRule type="expression" dxfId="10" priority="8">
+      <formula>AND($S9=0, $T9&lt;&gt;0)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="9">
+      <formula>AND($S9&lt;&gt;0, $T9=0)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T9:U9">
-    <cfRule type="expression" dxfId="7" priority="5">
-      <formula>AND($T9=0, $U9&lt;&gt;0)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="6">
-      <formula>AND($T9&lt;&gt;0, $U9=0)</formula>
+  <conditionalFormatting sqref="U9:V9">
+    <cfRule type="expression" dxfId="8" priority="6">
+      <formula>AND($U9=0, $V9&lt;&gt;0)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="7">
+      <formula>AND($U9&lt;&gt;0, $V9=0)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V9:W9">
-    <cfRule type="expression" dxfId="5" priority="3">
-      <formula>AND($V9=0, $W9&lt;&gt;0)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="4" priority="4">
-      <formula>AND($V9&lt;&gt;0, $W9=0)</formula>
+  <conditionalFormatting sqref="W9:X9">
+    <cfRule type="expression" dxfId="6" priority="4">
+      <formula>AND($W9=0, $X9&lt;&gt;0)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="5">
+      <formula>AND($W9&lt;&gt;0, $X9=0)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X9:Y9">
-    <cfRule type="expression" dxfId="3" priority="1">
-      <formula>AND($X9=0, $Y9&lt;&gt;0)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="2">
-      <formula>AND($X9&lt;&gt;0, $Y9=0)</formula>
+  <conditionalFormatting sqref="Y9:Z9">
+    <cfRule type="expression" dxfId="4" priority="2">
+      <formula>AND($Y9=0, $Z9&lt;&gt;0)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="3">
+      <formula>AND($Y9&lt;&gt;0, $Z9=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="expression" dxfId="1" priority="16">
+    <cfRule type="expression" dxfId="2" priority="17">
       <formula>AND($G9="YES", $H9="No")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9:H9">
-    <cfRule type="expression" dxfId="0" priority="17">
-      <formula>AND($G9="No", $H9="No")</formula>
+    <cfRule type="expression" dxfId="1" priority="18">
+      <formula>AND($G9="No", $H9="Yes")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N9">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>($N9="No")</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="1" right="1" top="1" bottom="1" header="1" footer="1"/>

</xml_diff>

<commit_message>
105612 - Funding Claims Submission - Add Signed Column, tests, template changes.
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.Operations.Reports.Reports/Templates/FundingClaimsProviderSubmissionsReport1920Template.xlsx
+++ b/src/ESFA.DC.Operations.Reports.Reports/Templates/FundingClaimsProviderSubmissionsReport1920Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VSTS\DCT\DC-Operations-Reports\src\ESFA.DC.Operations.Reports.Reports\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76902557-6B85-4404-B434-7B70387444EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41CE388D-1FF2-42B3-99A3-A5176F562419}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>UKPRN</t>
   </si>
@@ -173,6 +173,12 @@
   </si>
   <si>
     <t>&amp;=FundingClaimsInfo.NoOfReturningUnexpectedProviders</t>
+  </si>
+  <si>
+    <t>Signed</t>
+  </si>
+  <si>
+    <t>&amp;=FundingClaimsInfo.FundingClaimsSubmissionsDetails.Signed</t>
   </si>
 </sst>
 </file>
@@ -360,7 +366,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -387,6 +393,23 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -402,18 +425,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="22" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -938,10 +949,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:Z9"/>
+  <dimension ref="B1:AA9"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -956,79 +967,82 @@
     <col min="8" max="8" width="1.42578125" customWidth="1"/>
     <col min="9" max="9" width="0" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="12.140625" customWidth="1"/>
-    <col min="11" max="11" width="9.85546875" customWidth="1"/>
-    <col min="12" max="12" width="0" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="13.140625" customWidth="1"/>
-    <col min="14" max="14" width="21.28515625" style="13" customWidth="1"/>
-    <col min="15" max="15" width="18.42578125" style="2" customWidth="1"/>
-    <col min="16" max="16" width="18" customWidth="1"/>
-    <col min="17" max="18" width="18" style="3" customWidth="1"/>
-    <col min="19" max="20" width="18" style="5" customWidth="1"/>
-    <col min="21" max="21" width="15.28515625" style="2" customWidth="1"/>
-    <col min="22" max="22" width="14.28515625" style="1" customWidth="1"/>
-    <col min="23" max="23" width="15.28515625" style="5" customWidth="1"/>
-    <col min="24" max="24" width="14.28515625" style="5" customWidth="1"/>
-    <col min="25" max="25" width="17.42578125" style="4" customWidth="1"/>
-    <col min="26" max="26" width="18" style="4" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" style="18" customWidth="1"/>
+    <col min="12" max="12" width="9.85546875" customWidth="1"/>
+    <col min="13" max="13" width="0" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="13.140625" customWidth="1"/>
+    <col min="15" max="15" width="21.28515625" style="13" customWidth="1"/>
+    <col min="16" max="16" width="18.42578125" style="2" customWidth="1"/>
+    <col min="17" max="17" width="18" customWidth="1"/>
+    <col min="18" max="19" width="18" style="3" customWidth="1"/>
+    <col min="20" max="21" width="18" style="5" customWidth="1"/>
+    <col min="22" max="22" width="15.28515625" style="2" customWidth="1"/>
+    <col min="23" max="23" width="14.28515625" style="1" customWidth="1"/>
+    <col min="24" max="24" width="15.28515625" style="5" customWidth="1"/>
+    <col min="25" max="25" width="14.28515625" style="5" customWidth="1"/>
+    <col min="26" max="26" width="17.42578125" style="4" customWidth="1"/>
+    <col min="27" max="27" width="18" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:26" ht="11.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:26" ht="23.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="23" t="s">
+    <row r="1" spans="2:27" ht="11.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:27" ht="23.85" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="24"/>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="24"/>
-      <c r="R2" s="24"/>
-      <c r="S2" s="24"/>
-      <c r="T2" s="24"/>
-      <c r="U2" s="24"/>
-      <c r="V2" s="24"/>
-      <c r="W2" s="24"/>
-      <c r="X2" s="24"/>
-      <c r="Y2"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="20"/>
+      <c r="R2" s="20"/>
+      <c r="S2" s="20"/>
+      <c r="T2" s="20"/>
+      <c r="U2" s="20"/>
+      <c r="V2" s="20"/>
+      <c r="W2" s="20"/>
+      <c r="X2" s="20"/>
+      <c r="Y2" s="20"/>
       <c r="Z2"/>
+      <c r="AA2"/>
     </row>
-    <row r="3" spans="2:26" s="6" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:27" s="6" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="25" t="s">
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="H3" s="25"/>
+      <c r="H3" s="21"/>
       <c r="I3" s="14"/>
-      <c r="J3" s="27" t="s">
+      <c r="J3" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="K3" s="27"/>
-      <c r="L3" s="27"/>
-      <c r="M3" s="27"/>
-      <c r="N3" s="14"/>
-      <c r="Q3" s="13"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="14"/>
+      <c r="R3" s="13"/>
     </row>
-    <row r="4" spans="2:26" s="6" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="25" t="s">
+    <row r="4" spans="2:27" s="6" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="D4" s="25"/>
+      <c r="D4" s="21"/>
       <c r="E4" s="7" t="s">
         <v>19</v>
       </c>
@@ -1038,13 +1052,14 @@
       <c r="G4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="N4" s="13"/>
+      <c r="K4" s="18"/>
+      <c r="O4" s="13"/>
     </row>
-    <row r="5" spans="2:26" s="6" customFormat="1" ht="23.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="25" t="s">
+    <row r="5" spans="2:27" s="6" customFormat="1" ht="23.85" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="D5" s="25"/>
+      <c r="D5" s="21"/>
       <c r="E5" s="7" t="s">
         <v>20</v>
       </c>
@@ -1054,206 +1069,213 @@
       <c r="G5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="J5" s="26" t="s">
+      <c r="J5" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="K5" s="26"/>
-      <c r="L5" s="26"/>
-      <c r="M5" s="26"/>
-      <c r="N5" s="7" t="s">
+      <c r="K5" s="22"/>
+      <c r="L5" s="22"/>
+      <c r="M5" s="22"/>
+      <c r="N5" s="22"/>
+      <c r="O5" s="7" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="2:26" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="2:26" ht="22.35" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="2:26" ht="51" x14ac:dyDescent="0.25">
-      <c r="B8" s="19" t="s">
+    <row r="6" spans="2:27" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="2:27" ht="22.35" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="2:27" ht="51" x14ac:dyDescent="0.25">
+      <c r="B8" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="21" t="s">
+      <c r="C8" s="29"/>
+      <c r="D8" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="E8" s="22"/>
-      <c r="F8" s="20"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="29"/>
       <c r="G8" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="H8" s="21" t="s">
+      <c r="H8" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="I8" s="22"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="21" t="s">
+      <c r="I8" s="31"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="L8" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="L8" s="22"/>
-      <c r="M8" s="20"/>
-      <c r="N8" s="12" t="s">
+      <c r="M8" s="31"/>
+      <c r="N8" s="29"/>
+      <c r="O8" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="O8" s="9" t="s">
+      <c r="P8" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="P8" s="9" t="s">
+      <c r="Q8" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="Q8" s="9" t="s">
+      <c r="R8" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="R8" s="9" t="s">
+      <c r="S8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="S8" s="9" t="s">
+      <c r="T8" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="T8" s="9" t="s">
+      <c r="U8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="U8" s="9" t="s">
+      <c r="V8" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="V8" s="9" t="s">
+      <c r="W8" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="W8" s="9" t="s">
+      <c r="X8" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="X8" s="9" t="s">
+      <c r="Y8" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="Y8" s="9" t="s">
+      <c r="Z8" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="Z8" s="9" t="s">
+      <c r="AA8" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:27" x14ac:dyDescent="0.25">
       <c r="C9" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="17"/>
-      <c r="F9" s="18"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="27"/>
       <c r="G9" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="H9" s="16" t="s">
+      <c r="H9" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="I9" s="17"/>
-      <c r="J9" s="18"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="27"/>
       <c r="K9" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="L9" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="L9" s="17"/>
-      <c r="M9" s="18"/>
-      <c r="N9" s="11" t="s">
+      <c r="M9" s="26"/>
+      <c r="N9" s="27"/>
+      <c r="O9" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="O9" s="10" t="s">
+      <c r="P9" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="P9" s="10" t="s">
+      <c r="Q9" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="Q9" s="10" t="s">
+      <c r="R9" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="R9" s="10" t="s">
+      <c r="S9" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="S9" s="10" t="s">
+      <c r="T9" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="T9" s="10" t="s">
+      <c r="U9" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="U9" s="10" t="s">
+      <c r="V9" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="V9" s="10" t="s">
+      <c r="W9" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="W9" s="10" t="s">
+      <c r="X9" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="X9" s="10" t="s">
+      <c r="Y9" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="Y9" s="10" t="s">
+      <c r="Z9" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="Z9" s="10" t="s">
+      <c r="AA9" s="10" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="C2:X2"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="J5:M5"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="J3:M3"/>
-    <mergeCell ref="D3:F3"/>
     <mergeCell ref="H9:J9"/>
-    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="L9:N9"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="D8:F8"/>
     <mergeCell ref="H8:J8"/>
-    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="L8:N8"/>
     <mergeCell ref="D9:F9"/>
+    <mergeCell ref="C2:Y2"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="J5:N5"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="J3:N3"/>
+    <mergeCell ref="D3:F3"/>
   </mergeCells>
-  <conditionalFormatting sqref="O9:P9">
+  <conditionalFormatting sqref="P9:Q9">
     <cfRule type="expression" dxfId="14" priority="12">
-      <formula>AND($O9=0, $P9&lt;&gt;0)</formula>
+      <formula>AND($P9=0, $Q9&lt;&gt;0)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="13" priority="13">
-      <formula>AND($O9&lt;&gt;0, $P9=0)</formula>
+      <formula>AND($P9&lt;&gt;0, $Q9=0)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q9:R9">
+  <conditionalFormatting sqref="R9:S9">
     <cfRule type="expression" dxfId="12" priority="10">
-      <formula>AND($Q9=0, $R9&lt;&gt;0)</formula>
+      <formula>AND($R9=0, $S9&lt;&gt;0)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="11" priority="11">
-      <formula>AND($Q9&lt;&gt;0, $R9=0)</formula>
+      <formula>AND($R9&lt;&gt;0, $S9=0)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S9:T9">
+  <conditionalFormatting sqref="T9:U9">
     <cfRule type="expression" dxfId="10" priority="8">
-      <formula>AND($S9=0, $T9&lt;&gt;0)</formula>
+      <formula>AND($T9=0, $U9&lt;&gt;0)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="9" priority="9">
-      <formula>AND($S9&lt;&gt;0, $T9=0)</formula>
+      <formula>AND($T9&lt;&gt;0, $U9=0)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U9:V9">
+  <conditionalFormatting sqref="V9:W9">
     <cfRule type="expression" dxfId="8" priority="6">
-      <formula>AND($U9=0, $V9&lt;&gt;0)</formula>
+      <formula>AND($V9=0, $W9&lt;&gt;0)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="7" priority="7">
-      <formula>AND($U9&lt;&gt;0, $V9=0)</formula>
+      <formula>AND($V9&lt;&gt;0, $W9=0)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W9:X9">
+  <conditionalFormatting sqref="X9:Y9">
     <cfRule type="expression" dxfId="6" priority="4">
-      <formula>AND($W9=0, $X9&lt;&gt;0)</formula>
+      <formula>AND($X9=0, $Y9&lt;&gt;0)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="5" priority="5">
-      <formula>AND($W9&lt;&gt;0, $X9=0)</formula>
+      <formula>AND($X9&lt;&gt;0, $Y9=0)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y9:Z9">
+  <conditionalFormatting sqref="Z9:AA9">
     <cfRule type="expression" dxfId="4" priority="2">
-      <formula>AND($Y9=0, $Z9&lt;&gt;0)</formula>
+      <formula>AND($Z9=0, $AA9&lt;&gt;0)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="3" priority="3">
-      <formula>AND($Y9&lt;&gt;0, $Z9=0)</formula>
+      <formula>AND($Z9&lt;&gt;0, $AA9=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
@@ -1266,9 +1288,9 @@
       <formula>AND($G9="No", $H9="Yes")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N9">
+  <conditionalFormatting sqref="O9">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>($N9="No")</formula>
+      <formula>($O9="No")</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="1" right="1" top="1" bottom="1" header="1" footer="1"/>

</xml_diff>

<commit_message>
105711 - Bug fix
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.Operations.Reports.Reports/Templates/FundingClaimsProviderSubmissionsReport1920Template.xlsx
+++ b/src/ESFA.DC.Operations.Reports.Reports/Templates/FundingClaimsProviderSubmissionsReport1920Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VSTS\DCT\DC-Operations-Reports\src\ESFA.DC.Operations.Reports.Reports\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41CE388D-1FF2-42B3-99A3-A5176F562419}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF2D93BC-59F7-4421-BE9E-80ABF416094C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -79,9 +79,6 @@
     <t>&amp;=FundingClaimsInfo.ReportRun</t>
   </si>
   <si>
-    <t>&amp;=FundingClaimsInfo.TotalNoOfProviders</t>
-  </si>
-  <si>
     <t>&amp;=FundingClaimsInfo.NoOfProvidersExpectedToReturn</t>
   </si>
   <si>
@@ -179,6 +176,9 @@
   </si>
   <si>
     <t>&amp;=FundingClaimsInfo.FundingClaimsSubmissionsDetails.Signed</t>
+  </si>
+  <si>
+    <t>&amp;=FundingClaimsInfo.TotalNoOfReturningProviders</t>
   </si>
 </sst>
 </file>
@@ -398,18 +398,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="22" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -425,6 +413,18 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -952,7 +952,7 @@
   <dimension ref="B1:AA9"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -986,130 +986,130 @@
   <sheetData>
     <row r="1" spans="2:27" ht="11.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:27" ht="23.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="20"/>
-      <c r="S2" s="20"/>
-      <c r="T2" s="20"/>
-      <c r="U2" s="20"/>
-      <c r="V2" s="20"/>
-      <c r="W2" s="20"/>
-      <c r="X2" s="20"/>
-      <c r="Y2" s="20"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="27"/>
+      <c r="Q2" s="27"/>
+      <c r="R2" s="27"/>
+      <c r="S2" s="27"/>
+      <c r="T2" s="27"/>
+      <c r="U2" s="27"/>
+      <c r="V2" s="27"/>
+      <c r="W2" s="27"/>
+      <c r="X2" s="27"/>
+      <c r="Y2" s="27"/>
       <c r="Z2"/>
       <c r="AA2"/>
     </row>
     <row r="3" spans="2:27" s="6" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="D3" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="H3" s="21"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" s="28"/>
       <c r="I3" s="14"/>
-      <c r="J3" s="23" t="s">
+      <c r="J3" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23"/>
-      <c r="M3" s="23"/>
-      <c r="N3" s="23"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="30"/>
+      <c r="M3" s="30"/>
+      <c r="N3" s="30"/>
       <c r="O3" s="14"/>
       <c r="R3" s="13"/>
     </row>
     <row r="4" spans="2:27" s="6" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" s="21"/>
+      <c r="C4" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="28"/>
       <c r="E4" s="7" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K4" s="18"/>
       <c r="O4" s="13"/>
     </row>
     <row r="5" spans="2:27" s="6" customFormat="1" ht="23.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" s="21"/>
+      <c r="C5" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="28"/>
       <c r="E5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="J5" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="G5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="J5" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="K5" s="22"/>
-      <c r="L5" s="22"/>
-      <c r="M5" s="22"/>
-      <c r="N5" s="22"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="29"/>
       <c r="O5" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="2:27" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="2:27" ht="22.35" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="2:27" ht="51" x14ac:dyDescent="0.25">
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="29"/>
-      <c r="D8" s="30" t="s">
+      <c r="C8" s="23"/>
+      <c r="D8" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="E8" s="31"/>
-      <c r="F8" s="29"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="23"/>
       <c r="G8" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="H8" s="30" t="s">
+      <c r="H8" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="I8" s="31"/>
-      <c r="J8" s="29"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="23"/>
       <c r="K8" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="L8" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="L8" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="M8" s="31"/>
-      <c r="N8" s="29"/>
+      <c r="M8" s="25"/>
+      <c r="N8" s="23"/>
       <c r="O8" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P8" s="9" t="s">
         <v>6</v>
@@ -1150,71 +1150,78 @@
     </row>
     <row r="9" spans="2:27" x14ac:dyDescent="0.25">
       <c r="C9" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="E9" s="20"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="26"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="10" t="s">
+      <c r="H9" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="H9" s="25" t="s">
+      <c r="I9" s="20"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="L9" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="I9" s="26"/>
-      <c r="J9" s="27"/>
-      <c r="K9" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="L9" s="25" t="s">
+      <c r="M9" s="20"/>
+      <c r="N9" s="21"/>
+      <c r="O9" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="P9" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="M9" s="26"/>
-      <c r="N9" s="27"/>
-      <c r="O9" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="P9" s="10" t="s">
+      <c r="Q9" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="Q9" s="10" t="s">
+      <c r="R9" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="R9" s="10" t="s">
+      <c r="S9" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="S9" s="10" t="s">
+      <c r="T9" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="T9" s="10" t="s">
+      <c r="U9" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="U9" s="10" t="s">
+      <c r="V9" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="V9" s="10" t="s">
+      <c r="W9" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="W9" s="10" t="s">
+      <c r="X9" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="X9" s="10" t="s">
+      <c r="Y9" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="Y9" s="10" t="s">
+      <c r="Z9" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="Z9" s="10" t="s">
+      <c r="AA9" s="10" t="s">
         <v>38</v>
-      </c>
-      <c r="AA9" s="10" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="C2:Y2"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="J5:N5"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="J3:N3"/>
+    <mergeCell ref="D3:F3"/>
     <mergeCell ref="H9:J9"/>
     <mergeCell ref="L9:N9"/>
     <mergeCell ref="B8:C8"/>
@@ -1222,13 +1229,6 @@
     <mergeCell ref="H8:J8"/>
     <mergeCell ref="L8:N8"/>
     <mergeCell ref="D9:F9"/>
-    <mergeCell ref="C2:Y2"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="J5:N5"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="J3:N3"/>
-    <mergeCell ref="D3:F3"/>
   </mergeCells>
   <conditionalFormatting sqref="P9:Q9">
     <cfRule type="expression" dxfId="14" priority="12">

</xml_diff>